<commit_message>
removed some lambda functions and local functions Split spreadsheets to two sheets fixed comment in notebook
</commit_message>
<xml_diff>
--- a/engine_test.xlsx
+++ b/engine_test.xlsx
@@ -7,12 +7,13 @@
     <workbookView xWindow="0" yWindow="140" windowWidth="13920" windowHeight="4950"/>
   </bookViews>
   <sheets>
-    <sheet name="Definition" sheetId="1" r:id="rId1"/>
+    <sheet name="Instrument Properties" sheetId="1" r:id="rId1"/>
+    <sheet name="Curve Properties" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Definition!$C$1:$L$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Instrument Properties'!$C$1:$L$45</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -211,24 +212,6 @@
     <t>LINEAR_CCZR</t>
   </si>
   <si>
-    <t>FcastCurveL</t>
-  </si>
-  <si>
-    <t>FcastCurveR</t>
-  </si>
-  <si>
-    <t>DiscCurveL</t>
-  </si>
-  <si>
-    <t>DiscCurveR</t>
-  </si>
-  <si>
-    <t>ConventionL</t>
-  </si>
-  <si>
-    <t>ConventionR</t>
-  </si>
-  <si>
     <t>USDLIBOR3M</t>
   </si>
   <si>
@@ -236,6 +219,24 @@
   </si>
   <si>
     <t>USD-USDOIS</t>
+  </si>
+  <si>
+    <t>Forecast Curve Left</t>
+  </si>
+  <si>
+    <t>Forecast Curve Right</t>
+  </si>
+  <si>
+    <t>Discount Curve Left</t>
+  </si>
+  <si>
+    <t>Discount Curve Right</t>
+  </si>
+  <si>
+    <t>Convention Left</t>
+  </si>
+  <si>
+    <t>Convention Right</t>
   </si>
 </sst>
 </file>
@@ -638,10 +639,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O103"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -649,21 +651,19 @@
     <col min="1" max="1" width="45.81640625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.1796875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="18.26953125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.54296875" customWidth="1"/>
-    <col min="14" max="14" width="26" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.1796875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -674,22 +674,22 @@
         <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>54</v>
@@ -700,26 +700,20 @@
       <c r="L1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="4" t="str">
         <f>CONCATENATE(B2,"__Deposit__3M")</f>
         <v>USDLIBOR3M__Deposit__3M</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>51</v>
@@ -745,26 +739,20 @@
       <c r="L2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="4" t="str">
         <f>CONCATENATE(B3,"__Future__",J3,"_",K3)</f>
         <v>USDLIBOR3M__Future__1F_3M</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>51</v>
@@ -790,26 +778,20 @@
       <c r="L3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="4" t="str">
         <f t="shared" ref="A4:A15" si="0">CONCATENATE(B4,"__Future__",J4,"_",K4)</f>
         <v>USDLIBOR3M__Future__2F_3M</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>51</v>
@@ -835,26 +817,20 @@
       <c r="L4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>USDLIBOR3M__Future__3F_3M</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>51</v>
@@ -881,19 +857,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:12">
       <c r="A6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>USDLIBOR3M__Future__4F_3M</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>51</v>
@@ -920,19 +896,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:12">
       <c r="A7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>USDLIBOR3M__Future__5F_3M</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>51</v>
@@ -959,19 +935,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:12">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>USDLIBOR3M__Future__6F_3M</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>51</v>
@@ -998,19 +974,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:12">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>USDLIBOR3M__Future__7F_3M</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>51</v>
@@ -1037,19 +1013,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:12">
       <c r="A10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>USDLIBOR3M__Future__8F_3M</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>51</v>
@@ -1076,19 +1052,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:12">
       <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>USDLIBOR3M__Future__9F_3M</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>51</v>
@@ -1115,19 +1091,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:12">
       <c r="A12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>USDLIBOR3M__Future__10F_3M</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>51</v>
@@ -1154,19 +1130,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:12">
       <c r="A13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>USDLIBOR3M__Future__11F_3M</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>51</v>
@@ -1193,19 +1169,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:12">
       <c r="A14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>USDLIBOR3M__Future__12F_3M</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>51</v>
@@ -1232,19 +1208,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:12">
       <c r="A15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>USDLIBOR3M__Future__13F_3M</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>51</v>
@@ -1271,31 +1247,31 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:12">
       <c r="A16" s="4" t="str">
         <f>CONCATENATE(B16,"__Swap__",K16)</f>
         <v>USDLIBOR3M__Swap__4Y</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H16" s="5" t="str">
-        <f t="shared" ref="H16:H39" si="1">D16</f>
+        <f t="shared" ref="H16:H47" si="1">D16</f>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I16" s="5" t="str">
@@ -1318,19 +1294,19 @@
         <v>USDLIBOR3M__Swap__5Y</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>51</v>
@@ -1359,19 +1335,19 @@
         <v>USDLIBOR3M__Swap__6Y</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>51</v>
@@ -1400,19 +1376,19 @@
         <v>USDLIBOR3M__Swap__7Y</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>51</v>
@@ -1441,19 +1417,19 @@
         <v>USDLIBOR3M__Swap__8Y</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>51</v>
@@ -1482,19 +1458,19 @@
         <v>USDLIBOR3M__Swap__9Y</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>51</v>
@@ -1523,19 +1499,19 @@
         <v>USDLIBOR3M__Swap__10Y</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>51</v>
@@ -1564,19 +1540,19 @@
         <v>USDLIBOR3M__Swap__11Y</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>51</v>
@@ -1605,19 +1581,19 @@
         <v>USDLIBOR3M__Swap__12Y</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>51</v>
@@ -1646,19 +1622,19 @@
         <v>USDLIBOR3M__Swap__13Y</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>51</v>
@@ -1687,19 +1663,19 @@
         <v>USDLIBOR3M__Swap__14Y</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>51</v>
@@ -1728,19 +1704,19 @@
         <v>USDLIBOR3M__Swap__15Y</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>51</v>
@@ -1769,19 +1745,19 @@
         <v>USDLIBOR3M__Swap__16Y</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>51</v>
@@ -1810,19 +1786,19 @@
         <v>USDLIBOR3M__Swap__17Y</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>51</v>
@@ -1851,19 +1827,19 @@
         <v>USDLIBOR3M__Swap__18Y</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>51</v>
@@ -1892,19 +1868,19 @@
         <v>USDLIBOR3M__Swap__19Y</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>51</v>
@@ -1933,19 +1909,19 @@
         <v>USDLIBOR3M__Swap__20Y</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>51</v>
@@ -1974,19 +1950,19 @@
         <v>USDLIBOR3M__Swap__25Y</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>51</v>
@@ -2015,19 +1991,19 @@
         <v>USDLIBOR3M__Swap__30Y</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>51</v>
@@ -2056,19 +2032,19 @@
         <v>USDLIBOR3M__Swap__35Y</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>51</v>
@@ -2097,19 +2073,19 @@
         <v>USDLIBOR3M__Swap__40Y</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>51</v>
@@ -2138,19 +2114,19 @@
         <v>USDLIBOR3M__Swap__45Y</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>51</v>
@@ -2179,19 +2155,19 @@
         <v>USDLIBOR3M__Swap__50Y</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>51</v>
@@ -2220,19 +2196,19 @@
         <v>USDLIBOR3M__Swap__60Y</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>51</v>
@@ -2261,25 +2237,25 @@
         <v>USDLIBOR3M__Swap__70Y</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H40" s="5" t="str">
-        <f>D40</f>
+        <f t="shared" si="1"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I40" s="5" t="str">
@@ -2302,25 +2278,25 @@
         <v>USD-USDOIS__TermDeposit__1B</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H41" s="5" t="str">
-        <f>D41</f>
+        <f t="shared" si="1"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I41" s="5" t="s">
@@ -2342,25 +2318,25 @@
         <v>USD-USDOIS__TermDeposit__1M</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H42" s="5" t="str">
-        <f t="shared" ref="H42:H73" si="5">D42</f>
+        <f t="shared" si="1"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I42" s="5" t="s">
@@ -2382,25 +2358,25 @@
         <v>USD-USDOIS__TermDeposit__2M</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H43" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I43" s="5" t="s">
@@ -2422,25 +2398,25 @@
         <v>USD-USDOIS__TermDeposit__3M</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H44" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I44" s="5" t="s">
@@ -2462,25 +2438,25 @@
         <v>USD-USDOIS__TermDeposit__6M</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H45" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I45" s="5" t="s">
@@ -2502,25 +2478,25 @@
         <v>USD-USDOIS__TermDeposit__1Y</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H46" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I46" s="5" t="s">
@@ -2542,25 +2518,25 @@
         <v>USD-USDOIS__TermDeposit__2Y</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H47" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I47" s="5" t="s">
@@ -2582,25 +2558,25 @@
         <v>USD-USDOIS__TermDeposit__3Y</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H48" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="H48:H79" si="5">D48</f>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I48" s="5" t="s">
@@ -2622,19 +2598,19 @@
         <v>USD-USDOIS__TermDeposit__4Y</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>51</v>
@@ -2662,19 +2638,19 @@
         <v>USD-USDOIS__TermDeposit__5Y</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>51</v>
@@ -2702,19 +2678,19 @@
         <v>USD-USDOIS__TermDeposit__6Y</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>51</v>
@@ -2742,19 +2718,19 @@
         <v>USD-USDOIS__TermDeposit__7Y</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>51</v>
@@ -2782,19 +2758,19 @@
         <v>USD-USDOIS__TermDeposit__8Y</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>51</v>
@@ -2822,19 +2798,19 @@
         <v>USD-USDOIS__TermDeposit__9Y</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>51</v>
@@ -2862,19 +2838,19 @@
         <v>USD-USDOIS__TermDeposit__10Y</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>51</v>
@@ -2902,19 +2878,19 @@
         <v>USD-USDOIS__TermDeposit__11Y</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>51</v>
@@ -2942,19 +2918,19 @@
         <v>USD-USDOIS__TermDeposit__12Y</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>51</v>
@@ -2982,19 +2958,19 @@
         <v>USD-USDOIS__TermDeposit__13Y</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>51</v>
@@ -3022,19 +2998,19 @@
         <v>USD-USDOIS__TermDeposit__14Y</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>51</v>
@@ -3062,19 +3038,19 @@
         <v>USD-USDOIS__TermDeposit__15Y</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>51</v>
@@ -3102,19 +3078,19 @@
         <v>USD-USDOIS__TermDeposit__16Y</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>51</v>
@@ -3142,19 +3118,19 @@
         <v>USD-USDOIS__TermDeposit__17Y</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>51</v>
@@ -3182,19 +3158,19 @@
         <v>USD-USDOIS__TermDeposit__18Y</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>51</v>
@@ -3222,19 +3198,19 @@
         <v>USD-USDOIS__TermDeposit__19Y</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>51</v>
@@ -3262,19 +3238,19 @@
         <v>USD-USDOIS__TermDeposit__20Y</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>51</v>
@@ -3302,19 +3278,19 @@
         <v>USD-USDOIS__TermDeposit__25Y</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>51</v>
@@ -3342,19 +3318,19 @@
         <v>USD-USDOIS__TermDeposit__30Y</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>51</v>
@@ -3382,19 +3358,19 @@
         <v>USD-USDOIS__TermDeposit__35Y</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>51</v>
@@ -3422,19 +3398,19 @@
         <v>USD-USDOIS__TermDeposit__40Y</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>51</v>
@@ -3462,19 +3438,19 @@
         <v>USD-USDOIS__TermDeposit__45Y</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>51</v>
@@ -3502,19 +3478,19 @@
         <v>USD-USDOIS__TermDeposit__50Y</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>51</v>
@@ -3542,19 +3518,19 @@
         <v>USD-USDOIS__TermDeposit__60Y</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>51</v>
@@ -3582,19 +3558,19 @@
         <v>USD-USDOIS__TermDeposit__70Y</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>51</v>
@@ -3622,25 +3598,25 @@
         <v>USDLIBOR6M__BasisSwap__3M</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H74" s="5" t="str">
-        <f t="shared" ref="H74:H103" si="6">D74</f>
+        <f t="shared" si="5"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I74" s="5" t="str">
@@ -3659,33 +3635,33 @@
     </row>
     <row r="75" spans="1:12">
       <c r="A75" s="7" t="str">
-        <f t="shared" ref="A75:A103" si="7">CONCATENATE(B75,"__BasisSwap__",K75)</f>
+        <f t="shared" ref="A75:A103" si="6">CONCATENATE(B75,"__BasisSwap__",K75)</f>
         <v>USDLIBOR6M__BasisSwap__6M</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H75" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I75" s="5" t="str">
-        <f t="shared" ref="I75:I103" si="8">E75</f>
+        <f t="shared" ref="I75:I103" si="7">E75</f>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J75" s="5" t="s">
@@ -3700,33 +3676,33 @@
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__1Y</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H76" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I76" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J76" s="5" t="s">
@@ -3741,33 +3717,33 @@
     </row>
     <row r="77" spans="1:12">
       <c r="A77" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__2Y</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H77" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I77" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J77" s="5" t="s">
@@ -3782,33 +3758,33 @@
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__3Y</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H78" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I78" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J78" s="5" t="s">
@@ -3823,33 +3799,33 @@
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__4Y</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H79" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I79" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J79" s="5" t="s">
@@ -3864,33 +3840,33 @@
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__5Y</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H80" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="H80:H103" si="8">D80</f>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I80" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J80" s="5" t="s">
@@ -3905,33 +3881,33 @@
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__6Y</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G81" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H81" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I81" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J81" s="5" t="s">
@@ -3946,33 +3922,33 @@
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__7Y</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H82" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I82" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J82" s="5" t="s">
@@ -3987,33 +3963,33 @@
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__8Y</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H83" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I83" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J83" s="5" t="s">
@@ -4028,33 +4004,33 @@
     </row>
     <row r="84" spans="1:12">
       <c r="A84" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__9Y</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H84" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I84" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J84" s="5" t="s">
@@ -4069,33 +4045,33 @@
     </row>
     <row r="85" spans="1:12">
       <c r="A85" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__10Y</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H85" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I85" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J85" s="5" t="s">
@@ -4110,33 +4086,33 @@
     </row>
     <row r="86" spans="1:12">
       <c r="A86" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__11Y</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H86" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I86" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J86" s="5" t="s">
@@ -4151,33 +4127,33 @@
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__12Y</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H87" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I87" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J87" s="5" t="s">
@@ -4192,33 +4168,33 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__13Y</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H88" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I88" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J88" s="5" t="s">
@@ -4233,33 +4209,33 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__14Y</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H89" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I89" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J89" s="5" t="s">
@@ -4274,33 +4250,33 @@
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__15Y</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H90" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I90" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J90" s="5" t="s">
@@ -4315,33 +4291,33 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__16Y</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H91" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I91" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J91" s="5" t="s">
@@ -4356,33 +4332,33 @@
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__17Y</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H92" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I92" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J92" s="5" t="s">
@@ -4397,33 +4373,33 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__18Y</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H93" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I93" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J93" s="5" t="s">
@@ -4438,33 +4414,33 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__19Y</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H94" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I94" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J94" s="5" t="s">
@@ -4479,33 +4455,33 @@
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__20Y</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G95" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H95" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I95" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J95" s="5" t="s">
@@ -4520,33 +4496,33 @@
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__25Y</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G96" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H96" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I96" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J96" s="5" t="s">
@@ -4561,33 +4537,33 @@
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__30Y</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G97" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H97" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I97" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J97" s="5" t="s">
@@ -4602,33 +4578,33 @@
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__35Y</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G98" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H98" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I98" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J98" s="5" t="s">
@@ -4643,33 +4619,33 @@
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__40Y</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G99" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H99" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I99" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J99" s="5" t="s">
@@ -4684,33 +4660,33 @@
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__45Y</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G100" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H100" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I100" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J100" s="5" t="s">
@@ -4725,33 +4701,33 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__50Y</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G101" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H101" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I101" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J101" s="5" t="s">
@@ -4766,33 +4742,33 @@
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__60Y</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G102" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H102" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I102" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J102" s="5" t="s">
@@ -4807,33 +4783,33 @@
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>USDLIBOR6M__BasisSwap__70Y</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G103" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H103" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>USDLIBOR3M</v>
       </c>
       <c r="I103" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>USDLIBOR6M</v>
       </c>
       <c r="J103" s="5" t="s">
@@ -4862,4 +4838,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="16" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Curve Builder Solve Stages
</commit_message>
<xml_diff>
--- a/engine_test.xlsx
+++ b/engine_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="13920" windowHeight="4950"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="13920" windowHeight="4950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instrument Properties" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="74">
   <si>
     <t>3M</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>Convention Right</t>
+  </si>
+  <si>
+    <t>Solve Stage</t>
   </si>
 </sst>
 </file>
@@ -335,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -345,6 +348,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,7 +650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
@@ -4856,47 +4865,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>